<commit_message>
Sample chged from 1998Jul28_Art3_TrapA_wk31 to 1998Jul29_Art3_TrapA_Wk31
</commit_message>
<xml_diff>
--- a/6_referenceseqs_metadata/PlatesGH_metadata/EI_form_SIF PRO1747_plates_G_H_qtys_loaded_20180218.xlsx
+++ b/6_referenceseqs_metadata/PlatesGH_metadata/EI_form_SIF PRO1747_plates_G_H_qtys_loaded_20180218.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Roslin_Greenland/2017/bulk_samples/ArcDyn_scripts/6_referenceseqs_metadata/PlatesGH_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD618CFC-DE13-5249-8423-DB8B79D4A8FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0754444-735B-D74F-B270-610D6EB8F895}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="edited" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="104" r:id="rId4"/>
+    <pivotCache cacheId="127" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -9169,7 +9169,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="104" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="127" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D197" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField dataField="1" showAll="0">
@@ -10531,8 +10531,8 @@
   <dimension ref="A1:T193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20586,7 +20586,7 @@
         <v>50</v>
       </c>
       <c r="O162" s="15">
-        <f t="shared" ref="O162:O193" si="10">N162-5</f>
+        <f t="shared" ref="O162:O181" si="10">N162-5</f>
         <v>45</v>
       </c>
       <c r="P162" s="15" t="s">

</xml_diff>